<commit_message>
Making plots for CERF
</commit_message>
<xml_diff>
--- a/Data/BMA_Human_Impacts_Master_Datasheet.xlsx
+++ b/Data/BMA_Human_Impacts_Master_Datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suzanneguy/R_Projects/MS_Thesis_Data_Analysis/MS_Thesis_Stats/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C662BF53-B734-544A-840F-DFC4A70A31D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C135E1-D42C-6947-BFFA-3941045189C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{7BEAF15F-6FC0-0D44-B38F-6423A5795855}"/>
   </bookViews>
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D21D032-2960-8249-92E9-4A9F79446343}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>